<commit_message>
Align opencode handoff flow and expand lesson 18 mentor assets
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\code\godot_study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B29F3D-ABFD-44D0-8D70-3955C3F48653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48261D7-E185-4FBB-AFF3-A73E63353558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20260206" sheetId="80" r:id="rId1"/>
-    <sheet name="固定用法" sheetId="12" r:id="rId2"/>
-    <sheet name="temp" sheetId="75" r:id="rId3"/>
+    <sheet name="20260218" sheetId="81" r:id="rId2"/>
+    <sheet name="20260219" sheetId="82" r:id="rId3"/>
+    <sheet name="固定用法" sheetId="12" r:id="rId4"/>
+    <sheet name="temp" sheetId="75" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="70">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -818,6 +820,498 @@
   </si>
   <si>
     <t>兼容的; 顺从</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>intersect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>ˌɪ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>əˈ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sekt/</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+交叉；相交</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>velocity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>/v</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>əˈ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>l</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>ɒ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>ə</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ti/</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>速度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sprite</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>/spra</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>ɪ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>t/</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小精灵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rectangle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>ˈ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rektæ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>ŋ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>ɡ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>l/</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>长方形</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>collision</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>/k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>əˈ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>l</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>ɪʒ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n/</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>碰撞</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>polygon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>ˈ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>ɒ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>l</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>ɪɡə</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n/</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多边形</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iterate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>ˈɪ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>ə</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>re</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>ɪ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>t/</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+迭代</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hazard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>ˈ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hæz</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>ə</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>d/</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>危险</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>refactor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重构</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -825,7 +1319,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -876,6 +1370,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -897,7 +1398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -939,17 +1440,61 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="39">
+  <dxfs count="63">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1141,33 +1686,45 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1360,6 +1917,125 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1372,9 +2048,180 @@
         <sz val="20"/>
         <color theme="1"/>
         <name val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1387,17 +2234,63 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <family val="2"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <name val="等线"/>
         <charset val="134"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1603,86 +2496,136 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A24CF6AD-9AF9-4ECF-BDD0-B84E6BB48408}" name="表1_8822" displayName="表1_8822" ref="A1:I11" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A24CF6AD-9AF9-4ECF-BDD0-B84E6BB48408}" name="表1_8822" displayName="表1_8822" ref="A1:I11" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
   <autoFilter ref="A1:I11" xr:uid="{0C79A950-6278-4E06-B1E4-75EA0EB6EBAC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G7">
     <sortCondition ref="A1:A7"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{B81C60A3-67ED-445B-AD7D-227A2C59EAB1}" name="序号" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{1482EDE1-0E5D-41AC-BAC2-35F87B07659C}" name="单词" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{12F2CC43-555C-4A4E-8864-42072E7675CD}" name="音标" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{3769BCC1-337D-4653-A982-35A8A0597FC5}" name="翻译" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{20693796-9122-4277-B035-A0A8DD75C044}" name="默写" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{9BCA7220-452A-4DA7-A580-9AD64592236C}" name="结果" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{B81C60A3-67ED-445B-AD7D-227A2C59EAB1}" name="序号" dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{1482EDE1-0E5D-41AC-BAC2-35F87B07659C}" name="单词" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{12F2CC43-555C-4A4E-8864-42072E7675CD}" name="音标" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{3769BCC1-337D-4653-A982-35A8A0597FC5}" name="翻译" dataDxfId="57"/>
+    <tableColumn id="5" xr3:uid="{20693796-9122-4277-B035-A0A8DD75C044}" name="默写" dataDxfId="56"/>
+    <tableColumn id="6" xr3:uid="{9BCA7220-452A-4DA7-A580-9AD64592236C}" name="结果" dataDxfId="55">
       <calculatedColumnFormula>IF(表1_8822[[#This Row],[单词]]=表1_8822[[#This Row],[默写]],"true","false")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{50292F66-0015-43D7-873B-4ED9811E6D35}" name="随机数" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{50292F66-0015-43D7-873B-4ED9811E6D35}" name="随机数" dataDxfId="54">
       <calculatedColumnFormula>RAND()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{83B61ED7-76AA-46D9-AFF2-D47F4850A75F}" name="错误次数" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{59258ECF-954E-4391-B4C8-BF686EC36249}" name="temp" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{83B61ED7-76AA-46D9-AFF2-D47F4850A75F}" name="错误次数" dataDxfId="53"/>
+    <tableColumn id="9" xr3:uid="{59258ECF-954E-4391-B4C8-BF686EC36249}" name="temp" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{50EA691E-B118-40BB-B648-49576C6D2C98}" name="表1_812" displayName="表1_812" ref="A1:I10" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
-  <autoFilter ref="A1:I10" xr:uid="{0C79A950-6278-4E06-B1E4-75EA0EB6EBAC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4E879BC8-4300-40F6-ABC6-D0632861B8D1}" name="表1_8823" displayName="表1_8823" ref="A1:I8" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+  <autoFilter ref="A1:I8" xr:uid="{0C79A950-6278-4E06-B1E4-75EA0EB6EBAC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G7">
     <sortCondition ref="A1:A7"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{883E554D-A772-437C-9E77-0678DBD178AD}" name="序号" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{2A42EAE3-DE9E-4D0D-A6D9-32C3033AC046}" name="词组" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{07D5FEF3-326D-4D70-8F69-7094125A05DC}" name="出处" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{0013C7DC-C7AF-45A7-A313-7A55B54E07BF}" name="翻译" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{C94B0E08-45E5-48A8-8701-08C409FF157E}" name="默写" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{841AE484-7662-42CF-808A-BA5C5F455969}" name="结果" dataDxfId="31">
-      <calculatedColumnFormula>IF(表1_812[[#This Row],[词组]]=表1_812[[#This Row],[默写]],"true","false")</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{5E269C68-90D8-46E5-AA3B-65CE3415FE80}" name="序号" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{8E66FCBA-D1E9-46C2-B7C2-66CE787E47C1}" name="单词" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{E6DD52A5-894F-4C64-A139-55ED976703A5}" name="音标" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{B1A06F0F-7385-423E-85AE-2915B951F33A}" name="翻译" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{8CFBA5E1-A718-4DA0-B557-D401CC375EAF}" name="默写" dataDxfId="45"/>
+    <tableColumn id="6" xr3:uid="{8B7F4C0B-3722-46E3-8406-DD57BCCA826B}" name="结果" dataDxfId="44">
+      <calculatedColumnFormula>IF(表1_8823[[#This Row],[单词]]=表1_8823[[#This Row],[默写]],"true","false")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{188EC8A1-2E20-4AEF-83AA-C6FA3E5C5A9B}" name="随机数" dataDxfId="30">
+    <tableColumn id="7" xr3:uid="{8AD5614A-1EE2-469C-9704-7682A1112903}" name="随机数" dataDxfId="43">
       <calculatedColumnFormula>RAND()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{90B30AA5-2268-4C42-A9D4-A6F72BCE9BF1}" name="错误次数" dataDxfId="29"/>
-    <tableColumn id="9" xr3:uid="{9087B70F-B10A-4B36-999E-E93709E8FE5E}" name="temp" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{1CAB7C8E-C9A5-44A7-BBB4-03A3E1B47A3A}" name="错误次数" dataDxfId="42"/>
+    <tableColumn id="9" xr3:uid="{AD5FF949-1484-40B1-A8B8-F189427912BE}" name="temp" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{140C10B6-5E18-4D02-B50F-811E8BC599BA}" name="表8_11126913" displayName="表8_11126913" ref="K6:L10" totalsRowShown="0" headerRowDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C0065477-D6F8-4B18-9D5D-458417702FA5}" name="表1_8824" displayName="表1_8824" ref="A1:I8" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+  <autoFilter ref="A1:I8" xr:uid="{0C79A950-6278-4E06-B1E4-75EA0EB6EBAC}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G7">
+    <sortCondition ref="A1:A7"/>
+  </sortState>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{C70DF79A-473D-42B0-9CF4-282F66332D8E}" name="序号" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{C29C1513-F31C-40FA-A795-CF17D641D618}" name="单词" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{6315386D-5F33-438F-8989-CF8A46BAD113}" name="音标" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{765CD049-2536-4A25-B2B2-E30380BA86D1}" name="翻译" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{6CAC1B8F-90AB-4D17-855A-05DE7DAD4EB9}" name="默写" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{5696FA63-92F7-444E-9C79-5BD7A2F8FB5F}" name="结果" dataDxfId="33">
+      <calculatedColumnFormula>IF(表1_8824[[#This Row],[单词]]=表1_8824[[#This Row],[默写]],"true","false")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{ACB41684-942C-48C8-87B9-DD2838C172C5}" name="随机数" dataDxfId="32">
+      <calculatedColumnFormula>RAND()</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{BCD122E1-8BD1-4A86-92D0-D26C6F8AE46A}" name="错误次数" dataDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{A4985714-3691-4A69-B956-10CE343DD830}" name="temp" dataDxfId="30"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{50EA691E-B118-40BB-B648-49576C6D2C98}" name="表1_812" displayName="表1_812" ref="A1:I10" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+  <autoFilter ref="A1:I10" xr:uid="{0C79A950-6278-4E06-B1E4-75EA0EB6EBAC}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G7">
+    <sortCondition ref="A1:A7"/>
+  </sortState>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{883E554D-A772-437C-9E77-0678DBD178AD}" name="序号" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{2A42EAE3-DE9E-4D0D-A6D9-32C3033AC046}" name="词组" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{07D5FEF3-326D-4D70-8F69-7094125A05DC}" name="出处" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{0013C7DC-C7AF-45A7-A313-7A55B54E07BF}" name="翻译" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{C94B0E08-45E5-48A8-8701-08C409FF157E}" name="默写" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{841AE484-7662-42CF-808A-BA5C5F455969}" name="结果" dataDxfId="22">
+      <calculatedColumnFormula>IF(表1_812[[#This Row],[词组]]=表1_812[[#This Row],[默写]],"true","false")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{188EC8A1-2E20-4AEF-83AA-C6FA3E5C5A9B}" name="随机数" dataDxfId="21">
+      <calculatedColumnFormula>RAND()</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{90B30AA5-2268-4C42-A9D4-A6F72BCE9BF1}" name="错误次数" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{9087B70F-B10A-4B36-999E-E93709E8FE5E}" name="temp" dataDxfId="19"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{140C10B6-5E18-4D02-B50F-811E8BC599BA}" name="表8_11126913" displayName="表8_11126913" ref="K6:L10" totalsRowShown="0" headerRowDxfId="18">
   <autoFilter ref="K6:L10" xr:uid="{7514FFE4-E5C7-4C61-8BA1-2AD190E7E7FC}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3C3BE2A0-5D83-47EA-B9D2-BACFB9879B92}" name="日期" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{4866E288-1C65-4D62-9C88-2C1F90A480DF}" name="错误数" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{3C3BE2A0-5D83-47EA-B9D2-BACFB9879B92}" name="日期" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{4866E288-1C65-4D62-9C88-2C1F90A480DF}" name="错误数" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="81" xr:uid="{73F6CB16-B5D2-4ED0-BF73-68FBDF964635}" name="表1_882" displayName="表1_882" ref="A1:I8" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="81" xr:uid="{73F6CB16-B5D2-4ED0-BF73-68FBDF964635}" name="表1_882" displayName="表1_882" ref="A1:I8" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:I8" xr:uid="{0C79A950-6278-4E06-B1E4-75EA0EB6EBAC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G7">
     <sortCondition ref="A1:A7"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{35E23C06-D669-40E9-BFB6-385958F71C49}" name="序号" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{8F67E226-901E-4B90-AD2A-A4EF5A9B1C82}" name="单词" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{04F79930-61E7-4440-8DE4-413852227479}" name="音标" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{6B9E0832-DCE4-49BC-8FCA-63F937A6FB70}" name="翻译" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{BFF78518-A1A4-4813-92E8-C39A4AB8516F}" name="默写" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{E536D12F-93BA-4E25-A20A-DAF6CBB172A8}" name="结果" dataDxfId="17">
+    <tableColumn id="1" xr3:uid="{35E23C06-D669-40E9-BFB6-385958F71C49}" name="序号" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{8F67E226-901E-4B90-AD2A-A4EF5A9B1C82}" name="单词" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{04F79930-61E7-4440-8DE4-413852227479}" name="音标" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{6B9E0832-DCE4-49BC-8FCA-63F937A6FB70}" name="翻译" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{BFF78518-A1A4-4813-92E8-C39A4AB8516F}" name="默写" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{E536D12F-93BA-4E25-A20A-DAF6CBB172A8}" name="结果" dataDxfId="8">
       <calculatedColumnFormula>IF(表1_882[[#This Row],[单词]]=表1_882[[#This Row],[默写]],"true","false")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{AF53FBC6-0A2B-4F4C-BBA0-927691298489}" name="随机数" dataDxfId="16">
+    <tableColumn id="7" xr3:uid="{AF53FBC6-0A2B-4F4C-BBA0-927691298489}" name="随机数" dataDxfId="7">
       <calculatedColumnFormula>RAND()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{BD2125E6-1273-49B8-99D7-DEE9948974B0}" name="错误次数" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{4828E1F7-E6FD-440F-B8EB-A1421BACF7D7}" name="temp" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{BD2125E6-1273-49B8-99D7-DEE9948974B0}" name="错误次数" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{4828E1F7-E6FD-440F-B8EB-A1421BACF7D7}" name="temp" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1953,8 +2896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3009CB-7A21-4938-B4F2-41B2914433F3}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.75" x14ac:dyDescent="0.4"/>
@@ -2022,7 +2965,7 @@
       </c>
       <c r="G2" s="8">
         <f t="shared" ref="G2:G8" ca="1" si="0">RAND()</f>
-        <v>0.33009284256925697</v>
+        <v>0.90818179279580047</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
@@ -2047,7 +2990,7 @@
       </c>
       <c r="G3" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>9.2582721160468284E-2</v>
+        <v>0.63983950296702796</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
@@ -2072,7 +3015,7 @@
       </c>
       <c r="G4" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28872737574024432</v>
+        <v>0.51104239482402791</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -2098,7 +3041,7 @@
       </c>
       <c r="G5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.97607047145255665</v>
+        <v>0.45422249274557003</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
@@ -2124,7 +3067,7 @@
       </c>
       <c r="G6" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.21268622952825245</v>
+        <v>0.22479445986745406</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
@@ -2151,7 +3094,7 @@
       </c>
       <c r="G7" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7347759116153505</v>
+        <v>0.63751784236440601</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
@@ -2178,7 +3121,7 @@
       </c>
       <c r="G8" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.72257641922630311</v>
+        <v>0.56286724126772569</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
@@ -2189,23 +3132,23 @@
       <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="8" t="s">
         <v>37</v>
       </c>
       <c r="E9" s="8"/>
-      <c r="F9" s="16" t="str">
+      <c r="F9" s="8" t="str">
         <f>IF(表1_8822[[#This Row],[单词]]=表1_8822[[#This Row],[默写]],"true","false")</f>
         <v>false</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="8">
         <f ca="1">RAND()</f>
-        <v>0.24087373582077398</v>
+        <v>0.12699843580070391</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
@@ -2214,23 +3157,23 @@
       <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E10" s="8"/>
-      <c r="F10" s="16" t="str">
+      <c r="F10" s="8" t="str">
         <f>IF(表1_8822[[#This Row],[单词]]=表1_8822[[#This Row],[默写]],"true","false")</f>
         <v>false</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10" s="8">
         <f ca="1">RAND()</f>
-        <v>0.54623015182323986</v>
+        <v>5.3109099592897002E-2</v>
       </c>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
@@ -2239,23 +3182,23 @@
       <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E11" s="8"/>
-      <c r="F11" s="16" t="str">
+      <c r="F11" s="8" t="str">
         <f>IF(表1_8822[[#This Row],[单词]]=表1_8822[[#This Row],[默写]],"true","false")</f>
         <v>false</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="8">
         <f ca="1">RAND()</f>
-        <v>0.52213910192236634</v>
+        <v>0.75491275553023662</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
@@ -2270,7 +3213,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="false">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="false">
       <formula>NOT(ISERROR(SEARCH("false",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2282,6 +3225,488 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4551A3A0-EBBB-4769-9E86-6E6968E46984}">
+  <dimension ref="A1:L13"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="24.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="17" style="3" customWidth="1"/>
+    <col min="2" max="2" width="25.875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="24.625" customWidth="1"/>
+    <col min="4" max="4" width="32.875" customWidth="1"/>
+    <col min="5" max="5" width="30.375" customWidth="1"/>
+    <col min="6" max="6" width="14.125" customWidth="1"/>
+    <col min="7" max="7" width="11.125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5" customWidth="1"/>
+    <col min="9" max="9" width="21.875" customWidth="1"/>
+    <col min="10" max="10" width="18.25" customWidth="1"/>
+    <col min="11" max="11" width="23.125" style="10" customWidth="1"/>
+    <col min="12" max="12" width="22.375" style="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7" t="str">
+        <f>IF(表1_8823[[#This Row],[单词]]=表1_8823[[#This Row],[默写]],"true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="G2" s="8">
+        <f t="shared" ref="G2:G8" ca="1" si="0">RAND()</f>
+        <v>0.70969879882816644</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:12" ht="30.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7" t="str">
+        <f>IF(表1_8823[[#This Row],[单词]]=表1_8823[[#This Row],[默写]],"true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="G3" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>9.164694226922887E-2</v>
+      </c>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:12" ht="30.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7" t="str">
+        <f>IF(表1_8823[[#This Row],[单词]]=表1_8823[[#This Row],[默写]],"true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="G4" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>6.0861908706993373E-2</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="L4" s="11"/>
+    </row>
+    <row r="5" spans="1:12" ht="30.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7" t="str">
+        <f>IF(表1_8823[[#This Row],[单词]]=表1_8823[[#This Row],[默写]],"true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="G5" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.36341367346398468</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="L5" s="11"/>
+    </row>
+    <row r="6" spans="1:12" ht="30.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7" t="str">
+        <f>IF(表1_8823[[#This Row],[单词]]=表1_8823[[#This Row],[默写]],"true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="G6" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.4694283353152713E-3</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" ht="30.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7" t="str">
+        <f>IF(表1_8823[[#This Row],[单词]]=表1_8823[[#This Row],[默写]],"true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="G7" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.74707016439085894</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" ht="30.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8" t="str">
+        <f>IF(表1_8823[[#This Row],[单词]]=表1_8823[[#This Row],[默写]],"true","false")</f>
+        <v>true</v>
+      </c>
+      <c r="G8" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.2519031944490937</v>
+      </c>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K13:L13"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="false">
+      <formula>NOT(ISERROR(SEARCH("false",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAF080F2-2EA3-4BDD-99FF-905E689F8027}">
+  <dimension ref="A1:L13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="24.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="17" style="3" customWidth="1"/>
+    <col min="2" max="2" width="25.875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="24.625" customWidth="1"/>
+    <col min="4" max="4" width="32.875" customWidth="1"/>
+    <col min="5" max="5" width="30.375" customWidth="1"/>
+    <col min="6" max="6" width="14.125" customWidth="1"/>
+    <col min="7" max="7" width="11.125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5" customWidth="1"/>
+    <col min="9" max="9" width="21.875" customWidth="1"/>
+    <col min="10" max="10" width="18.25" customWidth="1"/>
+    <col min="11" max="11" width="23.125" style="10" customWidth="1"/>
+    <col min="12" max="12" width="22.375" style="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7" t="str">
+        <f>IF(表1_8824[[#This Row],[单词]]=表1_8824[[#This Row],[默写]],"true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="G2" s="8">
+        <f t="shared" ref="G2:G8" ca="1" si="0">RAND()</f>
+        <v>3.7689084768694814E-2</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:12" ht="30.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7" t="str">
+        <f>IF(表1_8824[[#This Row],[单词]]=表1_8824[[#This Row],[默写]],"true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="G3" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.19836298996293666</v>
+      </c>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:12" ht="30.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7" t="str">
+        <f>IF(表1_8824[[#This Row],[单词]]=表1_8824[[#This Row],[默写]],"true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="G4" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.40788986153903395</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="L4" s="11"/>
+    </row>
+    <row r="5" spans="1:12" ht="30.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7" t="str">
+        <f>IF(表1_8824[[#This Row],[单词]]=表1_8824[[#This Row],[默写]],"true","false")</f>
+        <v>true</v>
+      </c>
+      <c r="G5" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.24153380548180903</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="L5" s="11"/>
+    </row>
+    <row r="6" spans="1:12" ht="30.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7" t="str">
+        <f>IF(表1_8824[[#This Row],[单词]]=表1_8824[[#This Row],[默写]],"true","false")</f>
+        <v>true</v>
+      </c>
+      <c r="G6" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.29516926204049321</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" ht="30.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7" t="str">
+        <f>IF(表1_8824[[#This Row],[单词]]=表1_8824[[#This Row],[默写]],"true","false")</f>
+        <v>true</v>
+      </c>
+      <c r="G7" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.27725672016700187</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" ht="30.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8" t="str">
+        <f>IF(表1_8824[[#This Row],[单词]]=表1_8824[[#This Row],[默写]],"true","false")</f>
+        <v>true</v>
+      </c>
+      <c r="G8" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.28966326295465106</v>
+      </c>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K13:L13"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="false">
+      <formula>NOT(ISERROR(SEARCH("false",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{444C6FA9-0F19-43A9-B665-D4D7A704CE21}">
   <dimension ref="A1:L10"/>
   <sheetViews>
@@ -2348,7 +3773,7 @@
       </c>
       <c r="G2" s="8">
         <f t="shared" ref="G2:G10" ca="1" si="0">RAND()</f>
-        <v>0.34740249938411105</v>
+        <v>0.21699578364528804</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
@@ -2367,7 +3792,7 @@
       </c>
       <c r="G3" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1880876169998702E-2</v>
+        <v>0.99462058173876799</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
@@ -2389,7 +3814,7 @@
       </c>
       <c r="G4" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.40732036182318609</v>
+        <v>0.65780553041923728</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -2409,7 +3834,7 @@
       </c>
       <c r="G5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.90410164881934718</v>
+        <v>0.22179580640874563</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
@@ -2429,7 +3854,7 @@
       </c>
       <c r="G6" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>8.6679238960824745E-2</v>
+        <v>0.66496321559032734</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
@@ -2454,7 +3879,7 @@
       </c>
       <c r="G7" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.25454607188798606</v>
+        <v>0.7697173741371488</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
@@ -2475,7 +3900,7 @@
       </c>
       <c r="G8" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.37473779160748522</v>
+        <v>0.79645909414095006</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
@@ -2496,7 +3921,7 @@
       </c>
       <c r="G9" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.78543231949759085</v>
+        <v>0.82499500409128845</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
@@ -2517,7 +3942,7 @@
       </c>
       <c r="G10" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.8558436129550816</v>
+        <v>0.57221071667361378</v>
       </c>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
@@ -2527,7 +3952,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="13" priority="1" operator="containsText" text="false">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="false">
       <formula>NOT(ISERROR(SEARCH("false",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2539,7 +3964,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69945E7-0F8C-4DD6-8201-C2822A17A2C9}">
   <dimension ref="A1:L13"/>
   <sheetViews>
@@ -2606,7 +4031,7 @@
       </c>
       <c r="G2" s="8">
         <f t="shared" ref="G2:G8" ca="1" si="0">RAND()</f>
-        <v>0.90761223474410579</v>
+        <v>0.20282527842498987</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
@@ -2625,7 +4050,7 @@
       </c>
       <c r="G3" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49567420789194938</v>
+        <v>0.75275432730004854</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
@@ -2644,7 +4069,7 @@
       </c>
       <c r="G4" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9827901590462336E-3</v>
+        <v>0.51661883656846941</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -2664,7 +4089,7 @@
       </c>
       <c r="G5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.27052469637055621</v>
+        <v>0.961335500219345</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
@@ -2684,7 +4109,7 @@
       </c>
       <c r="G6" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.19599125790926963</v>
+        <v>0.25499774082597348</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
@@ -2705,7 +4130,7 @@
       </c>
       <c r="G7" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.26809245803438941</v>
+        <v>0.99662652055861523</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
@@ -2726,7 +4151,7 @@
       </c>
       <c r="G8" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.89765747026660181</v>
+        <v>0.76960014985292291</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
@@ -2743,7 +4168,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="false">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="false">
       <formula>NOT(ISERROR(SEARCH("false",F1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>